<commit_message>
Fixed Fiber column duplication
</commit_message>
<xml_diff>
--- a/temp/temp.xlsx
+++ b/temp/temp.xlsx
@@ -572,9 +572,7 @@
       <c r="O2" t="n">
         <v>2701</v>
       </c>
-      <c r="P2" t="n">
-        <v>2701</v>
-      </c>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr">
@@ -627,9 +625,7 @@
       <c r="O3" t="n">
         <v>2305</v>
       </c>
-      <c r="P3" t="n">
-        <v>2305</v>
-      </c>
+      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
           <t>VIOLATION-catv is 27" from drip_loop
@@ -688,9 +684,7 @@
       <c r="O4" t="n">
         <v>2304</v>
       </c>
-      <c r="P4" t="n">
-        <v>2304</v>
-      </c>
+      <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
           <t>VIOLATION-fiber is 29" from drip_loop
@@ -752,9 +746,7 @@
       <c r="O5" t="n">
         <v>2102</v>
       </c>
-      <c r="P5" t="n">
-        <v>2102</v>
-      </c>
+      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
           <t>VIOLATION-fiber is 24" from drip_loop
@@ -814,9 +806,7 @@
       <c r="O6" t="n">
         <v>2305</v>
       </c>
-      <c r="P6" t="n">
-        <v>2305</v>
-      </c>
+      <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
           <t>VIOLATION-fiber is 39" from neutral_height
@@ -877,9 +867,7 @@
       <c r="O7" t="n">
         <v>2606</v>
       </c>
-      <c r="P7" t="n">
-        <v>2606</v>
-      </c>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
           <t>VIOLATION-fiber is 26" from drip_loop
@@ -940,9 +928,7 @@
       <c r="O8" t="n">
         <v>2403</v>
       </c>
-      <c r="P8" t="n">
-        <v>2403</v>
-      </c>
+      <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
           <t>VIOLATION-catv is 11" from fiber</t>
@@ -999,9 +985,7 @@
       <c r="O9" t="n">
         <v>2511</v>
       </c>
-      <c r="P9" t="n">
-        <v>2511</v>
-      </c>
+      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
           <t>VIOLATION-fiber is 39" from drip_loop

</xml_diff>